<commit_message>
Added JP SelfBilling; TICC-254
</commit_message>
<xml_diff>
--- a/work-in-progress/Peppol Code Lists - Document types v8.5.xlsx
+++ b/work-in-progress/Peppol Code Lists - Document types v8.5.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\git-peppol\peppol-edec-codelists\work-in-progress\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\git-peppol\edec-codelists\work-in-progress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89D609B0-EA5A-4E14-86B8-0DE89AEB67BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC70BF79-DBA9-4789-9ACE-0F1043576911}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="525" windowWidth="27135" windowHeight="19170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1080" yWindow="1080" windowWidth="26715" windowHeight="14745" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Document Type" sheetId="5" r:id="rId1"/>
@@ -27,11 +27,22 @@
     <definedName name="_ftnref4" localSheetId="0">'Document Type'!$A$4</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1473" uniqueCount="542">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1489" uniqueCount="549">
   <si>
     <t>urn:oasis:names:specification:ubl:schema:xsd:ApplicationResponse-2::ApplicationResponse##urn:www.cenbii.eu:transaction:biicoretrdm057:ver1.0:#urn:www.peppol.eu:bis:peppol1a:ver1.0::2.0</t>
   </si>
@@ -1696,6 +1707,27 @@
   </si>
   <si>
     <t>urn:oasis:names:specification:ubl:schema:xsd:Enquiry-2::Enquiry##urn:fdc:peppol.eu:prac:trns:t009:1.0::2.2</t>
+  </si>
+  <si>
+    <t>JP BIS Self-Billing Invoice</t>
+  </si>
+  <si>
+    <t>JP BIS Self-Billing Credit Note</t>
+  </si>
+  <si>
+    <t>urn:oasis:names:specification:ubl:schema:xsd:Invoice-2::Invoice##urn:peppol:pint:selfbilling-1@jp-1::2.1</t>
+  </si>
+  <si>
+    <t>8.5</t>
+  </si>
+  <si>
+    <t>urn:oasis:names:specification:ubl:schema:xsd:CreditNote-2::CreditNote##urn:peppol:pint:selfbilling-1@jp-1::2.1</t>
+  </si>
+  <si>
+    <t>TICC-254</t>
+  </si>
+  <si>
+    <t>cenbii-procid-ubl::urn:peppol:bis:selfbilling</t>
   </si>
 </sst>
 </file>
@@ -2299,11 +2331,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F45987FB-91F4-488D-A9D3-2F3FAED3E07C}">
-  <dimension ref="A1:L196"/>
+  <dimension ref="A1:L198"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A121" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C131" sqref="C131"/>
+      <pane ySplit="1" topLeftCell="A187" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A198" sqref="A198"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15"/>
@@ -8368,6 +8400,66 @@
         <v>130</v>
       </c>
     </row>
+    <row r="197" spans="1:12">
+      <c r="A197" t="s">
+        <v>542</v>
+      </c>
+      <c r="B197" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C197" s="5" t="s">
+        <v>544</v>
+      </c>
+      <c r="D197" s="17" t="s">
+        <v>545</v>
+      </c>
+      <c r="E197" s="5" t="s">
+        <v>369</v>
+      </c>
+      <c r="H197" s="5" t="s">
+        <v>547</v>
+      </c>
+      <c r="I197" s="5" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="K197" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="L197" s="7" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="198" spans="1:12" ht="30">
+      <c r="A198" t="s">
+        <v>543</v>
+      </c>
+      <c r="B198" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C198" s="5" t="s">
+        <v>546</v>
+      </c>
+      <c r="D198" s="17" t="s">
+        <v>545</v>
+      </c>
+      <c r="E198" s="5" t="s">
+        <v>369</v>
+      </c>
+      <c r="H198" s="5" t="s">
+        <v>547</v>
+      </c>
+      <c r="I198" s="5" t="b">
+        <f>TRUE</f>
+        <v>1</v>
+      </c>
+      <c r="K198" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="L198" s="7" t="s">
+        <v>548</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:L190" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>